<commit_message>
added refactored requirements and architectural design files
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\An3Sem2\VVSS\Lab01\Lab01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\An3Sem2\VVSS\02_Inventory\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B36A810F-41C0-49DB-A430-A32635FAA780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{214C715E-CDDC-4101-87EC-E7B33E426EC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16395" yWindow="2760" windowWidth="18420" windowHeight="15375" tabRatio="650" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18195" yWindow="3780" windowWidth="18420" windowHeight="15375" tabRatio="650" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="76">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -173,9 +173,6 @@
     <t>There is no information about how the application should be initialized</t>
   </si>
   <si>
-    <t>The functionalities are defined properly</t>
-  </si>
-  <si>
     <t>The big picture of the clients needs is adequate</t>
   </si>
   <si>
@@ -249,13 +246,28 @@
   </si>
   <si>
     <t>What's up with the Inventory class and its logic?</t>
+  </si>
+  <si>
+    <t>The search should look only for the first appearance of the keyword, in the order in which the entities are shown</t>
+  </si>
+  <si>
+    <t>It's not specified what should happen with a product when a component it contains is deleted</t>
+  </si>
+  <si>
+    <t>The Inventory class manages both parts and products, so it does not respect the Single Responsibility principle. This is the case for the InventoryRepository class as well</t>
+  </si>
+  <si>
+    <t>When completing fields for adding parts, "Form contains blank field" error is shown when inputing a string instead of a number even though it should say something like "wrong data type</t>
+  </si>
+  <si>
+    <t>C08</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -339,6 +351,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF242424"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -440,7 +458,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -471,6 +489,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -513,7 +532,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -857,8 +878,8 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="I3:J5"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,19 +899,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
         <v>30</v>
@@ -903,7 +924,7 @@
       <c r="H3" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="36" t="s">
+      <c r="I3" s="22" t="s">
         <v>33</v>
       </c>
       <c r="J3" s="18">
@@ -914,14 +935,14 @@
       <c r="C4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="25"/>
+      <c r="E4" s="26"/>
       <c r="H4" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="36" t="s">
+      <c r="I4" s="22" t="s">
         <v>34</v>
       </c>
       <c r="J4" s="3">
@@ -932,14 +953,14 @@
       <c r="C5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="27"/>
+      <c r="E5" s="28"/>
       <c r="H5" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="36" t="s">
+      <c r="I5" s="22" t="s">
         <v>35</v>
       </c>
       <c r="J5" s="3">
@@ -951,15 +972,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
@@ -1026,7 +1047,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1036,12 +1057,12 @@
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="2" t="s">
-        <v>46</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
-        <f t="shared" si="0"/>
+        <f>B14+1</f>
         <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -1049,7 +1070,7 @@
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -1062,17 +1083,21 @@
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C17" s="1"/>
+      <c r="C17" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="D17" s="1"/>
-      <c r="E17" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
@@ -1177,8 +1202,8 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1197,19 +1222,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
         <v>30</v>
@@ -1222,7 +1247,7 @@
       <c r="H3" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="36" t="s">
+      <c r="I3" s="22" t="s">
         <v>33</v>
       </c>
       <c r="J3" s="18">
@@ -1233,14 +1258,14 @@
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="28"/>
+      <c r="E4" s="29"/>
       <c r="H4" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="36" t="s">
+      <c r="I4" s="22" t="s">
         <v>34</v>
       </c>
       <c r="J4" s="3">
@@ -1251,14 +1276,14 @@
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="30"/>
+      <c r="E5" s="31"/>
       <c r="H5" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="36" t="s">
+      <c r="I5" s="22" t="s">
         <v>35</v>
       </c>
       <c r="J5" s="3">
@@ -1270,15 +1295,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
@@ -1294,15 +1319,17 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
@@ -1310,11 +1337,11 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1323,11 +1350,11 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1336,12 +1363,10 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D13" s="1"/>
-      <c r="E13" s="2" t="s">
-        <v>60</v>
-      </c>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
@@ -1349,11 +1374,11 @@
         <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1362,11 +1387,11 @@
         <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1375,11 +1400,11 @@
         <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
@@ -1388,7 +1413,7 @@
         <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -1399,7 +1424,7 @@
         <v>9</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="2"/>
@@ -1410,7 +1435,7 @@
         <v>10</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -1421,11 +1446,11 @@
         <v>11</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
@@ -1513,8 +1538,8 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1534,19 +1559,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
         <v>30</v>
@@ -1559,7 +1584,7 @@
       <c r="H3" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="36" t="s">
+      <c r="I3" s="22" t="s">
         <v>33</v>
       </c>
       <c r="J3" s="18">
@@ -1570,14 +1595,14 @@
       <c r="C4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="31"/>
+      <c r="E4" s="32"/>
       <c r="H4" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="36" t="s">
+      <c r="I4" s="22" t="s">
         <v>34</v>
       </c>
       <c r="J4" s="3">
@@ -1588,14 +1613,14 @@
       <c r="C5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="33"/>
+      <c r="E5" s="34"/>
       <c r="H5" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="36" t="s">
+      <c r="I5" s="22" t="s">
         <v>35</v>
       </c>
       <c r="J5" s="3">
@@ -1607,15 +1632,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
@@ -1636,23 +1661,27 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:10" ht="82.5" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
+      <c r="E11" s="37" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
@@ -1732,13 +1761,13 @@
         <v>11</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
@@ -1863,7 +1892,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="I3:J5"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1884,19 +1913,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
         <v>30</v>
@@ -1909,7 +1938,7 @@
       <c r="H3" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="36" t="s">
+      <c r="I3" s="22" t="s">
         <v>33</v>
       </c>
       <c r="J3" s="18">
@@ -1920,12 +1949,12 @@
       <c r="C4" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
       <c r="H4" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="36" t="s">
+      <c r="I4" s="22" t="s">
         <v>34</v>
       </c>
       <c r="J4" s="3">
@@ -1936,12 +1965,12 @@
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
       <c r="H5" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="36" t="s">
+      <c r="I5" s="22" t="s">
         <v>35</v>
       </c>
       <c r="J5" s="3">
@@ -1953,8 +1982,8 @@
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
       <c r="F6" s="21"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -2187,11 +2216,11 @@
       <c r="E31" s="11"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C32" s="34" t="s">
+      <c r="C32" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="35"/>
-      <c r="E32" s="35"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="36"/>
       <c r="F32" s="19"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated nomber of hours for solarLint
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -314,7 +314,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -392,13 +392,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <i val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -488,7 +481,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -598,10 +591,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -697,12 +686,12 @@
       <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="16.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="41.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="41.41"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="6" style="1" width="8.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="24.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.43"/>
@@ -1029,12 +1018,12 @@
       <selection pane="topLeft" activeCell="H19" activeCellId="0" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="16.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="41.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="41.41"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="6" style="1" width="8.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="22.01"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="10" style="1" width="8.86"/>
@@ -1365,17 +1354,17 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="41.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="41.41"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="6" style="1" width="8.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="26.71"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="10" style="1" width="8.86"/>
@@ -1726,11 +1715,11 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I14" activeCellId="0" sqref="I14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I28" activeCellId="0" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.29"/>
@@ -1902,7 +1891,7 @@
       <c r="E13" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="F13" s="28" t="s">
+      <c r="F13" s="16" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2088,12 +2077,14 @@
       <c r="E31" s="18"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="29" t="s">
+      <c r="C32" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="D32" s="29"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="30"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="29" t="n">
+        <v>0.5</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>